<commit_message>
Fix CSV signal generation to match GenX Gold Master EA structure
- Update `demo_excel_generator.py` to include "Confidence" column in MT4 CSV output (index 7).
- Update `MT4_GenX_EA_Example.mq4` to read the "Confidence" column, maintaining compatibility.
- Add `verify_csv_structure.py` to ensure generated CSV matches the EA's expected schema.
- This ensures `GenX_Gold_Master_EA.mq4` receives the confidence values it relies on for risk management.
</commit_message>
<xml_diff>
--- a/signal_output/genx_signals.xlsx
+++ b/signal_output/genx_signals.xlsx
@@ -40,7 +40,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -51,18 +51,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFC7CE"/>
-        <bgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -84,14 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -460,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,90 +517,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:28</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>XAUAUD</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>4064.91481</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>4064.91121</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>4064.91896</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>84.0%</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:55</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>XAUGBP</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>2109.70362</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>2109.7061</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>2109.69605</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>84.0%</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -636,85 +537,85 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>GenX FX Trading Dashboard</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Total Signals</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Active Signals</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>BUY Signals</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>SELL Signals</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Average Confidence</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>83.5%</t>
+          <t>86.6%</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>Average Risk/Reward</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.93</t>
+          <t>2.12</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Last Update</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-07-28 21:07:35</t>
+          <t>2026-01-28 19:19:08</t>
         </is>
       </c>
     </row>
@@ -729,7 +630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,52 +639,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Symbol</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Signal</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Entry</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>TP</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Lots</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Confidence</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>R:R</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -792,12 +693,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-28 21:19</t>
+          <t>2026-01-28 19:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>XAUUSD</t>
+          <t>XAUCHF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -806,22 +707,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2638.81797</v>
+        <v>2347.93893</v>
       </c>
       <c r="E2" t="n">
-        <v>2638.81536</v>
+        <v>2347.93613</v>
       </c>
       <c r="F2" t="n">
-        <v>2638.82472</v>
+        <v>2347.94382</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="H2" t="n">
-        <v>0.91</v>
+        <v>0.8</v>
       </c>
       <c r="I2" t="n">
-        <v>2.59</v>
+        <v>1.75</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -832,36 +733,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-28 20:56</t>
+          <t>2026-01-28 18:53</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NZDUSD</t>
+          <t>XAUUSD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5863</v>
+        <v>2652.57639</v>
       </c>
       <c r="E3" t="n">
-        <v>0.58862</v>
+        <v>2652.57167</v>
       </c>
       <c r="F3" t="n">
-        <v>0.58136</v>
+        <v>2652.58378</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="H3" t="n">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="I3" t="n">
-        <v>2.12</v>
+        <v>1.56</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -872,36 +773,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-28 20:43</t>
+          <t>2026-01-28 19:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EURUSD</t>
+          <t>XAUEUR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.10395</v>
+        <v>2430.52918</v>
       </c>
       <c r="E4" t="n">
-        <v>1.10659</v>
+        <v>2430.52637</v>
       </c>
       <c r="F4" t="n">
-        <v>1.09987</v>
+        <v>2430.53709</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="H4" t="n">
-        <v>0.78</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>1.54</v>
+        <v>2.82</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -912,480 +813,80 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-28 20:54</t>
+          <t>2026-01-28 19:32</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>XAUCAD</t>
+          <t>USDCHF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3602.6381</v>
+        <v>0.88469</v>
       </c>
       <c r="E5" t="n">
-        <v>3602.64162</v>
+        <v>0.88245</v>
       </c>
       <c r="F5" t="n">
-        <v>3602.63223</v>
+        <v>0.89188</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H5" t="n">
         <v>0.85</v>
       </c>
       <c r="I5" t="n">
-        <v>1.67</v>
+        <v>3.21</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Filled</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-28 21:28</t>
+          <t>2026-01-28 19:15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>XAUAUD</t>
+          <t>AUDUSD</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4064.91481</v>
+        <v>0.65584</v>
       </c>
       <c r="E6" t="n">
-        <v>4064.91121</v>
+        <v>0.6591900000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>4064.91896</v>
+        <v>0.65158</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="I6" t="n">
-        <v>1.15</v>
+        <v>1.28</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:55</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>XAUGBP</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>2109.70362</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2109.7061</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2109.69605</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="I7" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:40</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>XAUCAD</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>3637.04486</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3637.0413</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3637.05461</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
           <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:33</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>XAUCHF</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>2330.19431</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2330.19843</v>
-      </c>
-      <c r="F9" t="n">
-        <v>2330.18961</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Filled</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:19</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>XAUUSD</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>2654.13881</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2654.13442</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2654.14534</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:52</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>XAUEUR</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>2414.83832</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2414.84059</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2414.82938</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="I11" t="n">
-        <v>3.94</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Filled</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:59</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>NZDUSD</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0.58938</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.59428</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.58413</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:25</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>EURUSD</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>1.10743</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1.10362</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.1122</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:30</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>XAUEUR</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>2412.942</v>
-      </c>
-      <c r="E14" t="n">
-        <v>2412.93763</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2412.94933</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="I14" t="n">
-        <v>1.68</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Filled</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:35</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>USDCAD</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1.3615</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1.36633</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1.35425</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:07</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>USDCHF</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>0.88156</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.87934</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.88597</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Filled</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix CSV signal generation to match GenX Gold Master EA structure (#42)
- Update `demo_excel_generator.py` to include "Confidence" column in MT4 CSV output (index 7).
- Update `MT4_GenX_EA_Example.mq4` to read the "Confidence" column, maintaining compatibility.
- Add `verify_csv_structure.py` to ensure generated CSV matches the EA's expected schema.
- This ensures `GenX_Gold_Master_EA.mq4` receives the confidence values it relies on for risk management.

Co-authored-by: google-labs-jules[bot] <161369871+google-labs-jules[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/signal_output/genx_signals.xlsx
+++ b/signal_output/genx_signals.xlsx
@@ -40,7 +40,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -51,18 +51,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFC7CE"/>
-        <bgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -84,14 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -460,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,90 +517,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:28</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>XAUAUD</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>4064.91481</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>4064.91121</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>4064.91896</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>84.0%</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:55</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>XAUGBP</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>2109.70362</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>2109.7061</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>2109.69605</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>84.0%</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -636,85 +537,85 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>GenX FX Trading Dashboard</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Total Signals</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Active Signals</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>BUY Signals</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>SELL Signals</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Average Confidence</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>83.5%</t>
+          <t>86.6%</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>Average Risk/Reward</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.93</t>
+          <t>2.12</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Last Update</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-07-28 21:07:35</t>
+          <t>2026-01-28 19:19:08</t>
         </is>
       </c>
     </row>
@@ -729,7 +630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,52 +639,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Symbol</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Signal</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Entry</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>TP</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Lots</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Confidence</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>R:R</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -792,12 +693,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-28 21:19</t>
+          <t>2026-01-28 19:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>XAUUSD</t>
+          <t>XAUCHF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -806,22 +707,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2638.81797</v>
+        <v>2347.93893</v>
       </c>
       <c r="E2" t="n">
-        <v>2638.81536</v>
+        <v>2347.93613</v>
       </c>
       <c r="F2" t="n">
-        <v>2638.82472</v>
+        <v>2347.94382</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="H2" t="n">
-        <v>0.91</v>
+        <v>0.8</v>
       </c>
       <c r="I2" t="n">
-        <v>2.59</v>
+        <v>1.75</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -832,36 +733,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-28 20:56</t>
+          <t>2026-01-28 18:53</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NZDUSD</t>
+          <t>XAUUSD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5863</v>
+        <v>2652.57639</v>
       </c>
       <c r="E3" t="n">
-        <v>0.58862</v>
+        <v>2652.57167</v>
       </c>
       <c r="F3" t="n">
-        <v>0.58136</v>
+        <v>2652.58378</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="H3" t="n">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="I3" t="n">
-        <v>2.12</v>
+        <v>1.56</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -872,36 +773,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-28 20:43</t>
+          <t>2026-01-28 19:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EURUSD</t>
+          <t>XAUEUR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.10395</v>
+        <v>2430.52918</v>
       </c>
       <c r="E4" t="n">
-        <v>1.10659</v>
+        <v>2430.52637</v>
       </c>
       <c r="F4" t="n">
-        <v>1.09987</v>
+        <v>2430.53709</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="H4" t="n">
-        <v>0.78</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>1.54</v>
+        <v>2.82</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -912,480 +813,80 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-28 20:54</t>
+          <t>2026-01-28 19:32</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>XAUCAD</t>
+          <t>USDCHF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3602.6381</v>
+        <v>0.88469</v>
       </c>
       <c r="E5" t="n">
-        <v>3602.64162</v>
+        <v>0.88245</v>
       </c>
       <c r="F5" t="n">
-        <v>3602.63223</v>
+        <v>0.89188</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H5" t="n">
         <v>0.85</v>
       </c>
       <c r="I5" t="n">
-        <v>1.67</v>
+        <v>3.21</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Filled</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-28 21:28</t>
+          <t>2026-01-28 19:15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>XAUAUD</t>
+          <t>AUDUSD</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4064.91481</v>
+        <v>0.65584</v>
       </c>
       <c r="E6" t="n">
-        <v>4064.91121</v>
+        <v>0.6591900000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>4064.91896</v>
+        <v>0.65158</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="I6" t="n">
-        <v>1.15</v>
+        <v>1.28</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:55</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>XAUGBP</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>2109.70362</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2109.7061</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2109.69605</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="I7" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:40</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>XAUCAD</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>3637.04486</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3637.0413</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3637.05461</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
           <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:33</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>XAUCHF</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>2330.19431</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2330.19843</v>
-      </c>
-      <c r="F9" t="n">
-        <v>2330.18961</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Filled</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:19</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>XAUUSD</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>2654.13881</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2654.13442</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2654.14534</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:52</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>XAUEUR</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>2414.83832</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2414.84059</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2414.82938</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="I11" t="n">
-        <v>3.94</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Filled</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2025-07-28 20:59</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>NZDUSD</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0.58938</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.59428</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.58413</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:25</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>EURUSD</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>1.10743</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1.10362</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.1122</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:30</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>XAUEUR</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>2412.942</v>
-      </c>
-      <c r="E14" t="n">
-        <v>2412.93763</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2412.94933</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="I14" t="n">
-        <v>1.68</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Filled</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:35</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>USDCAD</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1.3615</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1.36633</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1.35425</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-07-28 21:07</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>USDCHF</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>0.88156</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.87934</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.88597</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Filled</t>
         </is>
       </c>
     </row>

</xml_diff>